<commit_message>
- Added charter - Added adx-13
</commit_message>
<xml_diff>
--- a/docs/examples/Jo.Tests.Indicators/intc-adx-13.xlsx
+++ b/docs/examples/Jo.Tests.Indicators/intc-adx-13.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyDev\Github\tenwinds.Stock.Indicators\docs\examples\Jo.Tests.Indicators\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82A7635A-404B-4183-B215-4AFFE9830B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{377AF7DD-58C1-470E-A941-5EE9EA4C8715}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="intc-adx-13" sheetId="1" r:id="rId1"/>
@@ -4132,7 +4132,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.7387662235526304E-2"/>
+          <c:y val="0.11791737408036222"/>
+          <c:w val="0.9416698918475086"/>
+          <c:h val="0.7277927355854712"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -8731,16 +8741,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>550545</xdr:colOff>
+      <xdr:row>332</xdr:row>
+      <xdr:rowOff>43815</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>47624</xdr:colOff>
-      <xdr:row>361</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>154304</xdr:colOff>
+      <xdr:row>363</xdr:row>
+      <xdr:rowOff>43815</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9073,12 +9083,13 @@
       <selection pane="bottomLeft" activeCell="B406" sqref="B406:D406"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9095,72 +9106,72 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>44085</v>
       </c>
     </row>
-    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>44088</v>
       </c>
     </row>
-    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>44089</v>
       </c>
     </row>
-    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>44090</v>
       </c>
     </row>
-    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>44091</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>44092</v>
       </c>
     </row>
-    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>44095</v>
       </c>
     </row>
-    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>44096</v>
       </c>
     </row>
-    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>44097</v>
       </c>
     </row>
-    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>44098</v>
       </c>
     </row>
-    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>44099</v>
       </c>
     </row>
-    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>44102</v>
       </c>
     </row>
-    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>44103</v>
       </c>
     </row>
-    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>44104</v>
       </c>
@@ -9171,7 +9182,7 @@
         <v>16.237593589184101</v>
       </c>
     </row>
-    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>44105</v>
       </c>
@@ -9182,7 +9193,7 @@
         <v>15.2253127426918</v>
       </c>
     </row>
-    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>44106</v>
       </c>
@@ -9193,7 +9204,7 @@
         <v>20.569509342530999</v>
       </c>
     </row>
-    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>44109</v>
       </c>
@@ -9204,7 +9215,7 @@
         <v>19.4587559859362</v>
       </c>
     </row>
-    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>44110</v>
       </c>
@@ -9215,7 +9226,7 @@
         <v>17.566846086492099</v>
       </c>
     </row>
-    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>44111</v>
       </c>
@@ -9226,7 +9237,7 @@
         <v>15.832606286953499</v>
       </c>
     </row>
-    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>44112</v>
       </c>
@@ -9237,7 +9248,7 @@
         <v>14.886237992021799</v>
       </c>
     </row>
-    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>44113</v>
       </c>
@@ -9248,7 +9259,7 @@
         <v>13.732142326130999</v>
       </c>
     </row>
-    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>44116</v>
       </c>
@@ -9259,7 +9270,7 @@
         <v>12.503623034947401</v>
       </c>
     </row>
-    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>44117</v>
       </c>
@@ -9270,7 +9281,7 @@
         <v>11.941230196569901</v>
       </c>
     </row>
-    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>44118</v>
       </c>
@@ -9281,7 +9292,7 @@
         <v>11.9691643201402</v>
       </c>
     </row>
-    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>44119</v>
       </c>
@@ -9292,7 +9303,7 @@
         <v>16.848450638746399</v>
       </c>
     </row>
-    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>44120</v>
       </c>
@@ -9306,7 +9317,7 @@
         <v>29.350802985999401</v>
       </c>
     </row>
-    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>44123</v>
       </c>
@@ -9320,7 +9331,7 @@
         <v>30.374823322327099</v>
       </c>
     </row>
-    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>44124</v>
       </c>
@@ -9334,7 +9345,7 @@
         <v>30.479120446261501</v>
       </c>
     </row>
-    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>44125</v>
       </c>
@@ -9348,7 +9359,7 @@
         <v>29.9542019332881</v>
       </c>
     </row>
-    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>44126</v>
       </c>
@@ -9362,7 +9373,7 @@
         <v>29.596293034473899</v>
       </c>
     </row>
-    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>44127</v>
       </c>
@@ -9376,7 +9387,7 @@
         <v>29.796501586910001</v>
       </c>
     </row>
-    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>44130</v>
       </c>
@@ -9390,7 +9401,7 @@
         <v>30.579204930087201</v>
       </c>
     </row>
-    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>44131</v>
       </c>
@@ -9404,7 +9415,7 @@
         <v>31.637886184525701</v>
       </c>
     </row>
-    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>44132</v>
       </c>
@@ -9418,7 +9429,7 @@
         <v>33.0136656466129</v>
       </c>
     </row>
-    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>44133</v>
       </c>
@@ -9432,7 +9443,7 @@
         <v>34.375970815895599</v>
       </c>
     </row>
-    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>44134</v>
       </c>
@@ -9446,7 +9457,7 @@
         <v>35.2966570113432</v>
       </c>
     </row>
-    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>44137</v>
       </c>
@@ -9460,7 +9471,7 @@
         <v>35.870068704430501</v>
       </c>
     </row>
-    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>44138</v>
       </c>
@@ -9477,7 +9488,7 @@
         <v>32.656729751590397</v>
       </c>
     </row>
-    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>44139</v>
       </c>
@@ -9494,7 +9505,7 @@
         <v>32.851336655428497</v>
       </c>
     </row>
-    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>44140</v>
       </c>
@@ -9511,7 +9522,7 @@
         <v>32.328851357850901</v>
       </c>
     </row>
-    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>44141</v>
       </c>
@@ -9528,7 +9539,7 @@
         <v>31.733655272222901</v>
       </c>
     </row>
-    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>44144</v>
       </c>
@@ -9545,7 +9556,7 @@
         <v>30.531423280138799</v>
       </c>
     </row>
-    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>44145</v>
       </c>
@@ -9562,7 +9573,7 @@
         <v>29.790905035794101</v>
       </c>
     </row>
-    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>44146</v>
       </c>
@@ -9579,7 +9590,7 @@
         <v>29.406297457632501</v>
       </c>
     </row>
-    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>44147</v>
       </c>
@@ -9596,7 +9607,7 @@
         <v>29.683134872529301</v>
       </c>
     </row>
-    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>44148</v>
       </c>
@@ -9613,7 +9624,7 @@
         <v>30.1379447152753</v>
       </c>
     </row>
-    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>44151</v>
       </c>
@@ -9630,7 +9641,7 @@
         <v>30.029303990990901</v>
       </c>
     </row>
-    <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>44152</v>
       </c>
@@ -9647,7 +9658,7 @@
         <v>29.912026539354301</v>
       </c>
     </row>
-    <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>44153</v>
       </c>
@@ -9664,7 +9675,7 @@
         <v>29.806477312424501</v>
       </c>
     </row>
-    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>44154</v>
       </c>
@@ -9681,7 +9692,7 @@
         <v>29.622398321228701</v>
       </c>
     </row>
-    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>44155</v>
       </c>
@@ -9698,7 +9709,7 @@
         <v>28.973432230748099</v>
       </c>
     </row>
-    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>44158</v>
       </c>
@@ -9715,7 +9726,7 @@
         <v>27.9057488498723</v>
       </c>
     </row>
-    <row r="54" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>44159</v>
       </c>
@@ -9732,7 +9743,7 @@
         <v>26.921319713150201</v>
       </c>
     </row>
-    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>44160</v>
       </c>
@@ -9749,7 +9760,7 @@
         <v>25.296480040398599</v>
       </c>
     </row>
-    <row r="56" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>44162</v>
       </c>
@@ -9766,7 +9777,7 @@
         <v>24.3239965387613</v>
       </c>
     </row>
-    <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>44165</v>
       </c>
@@ -9783,7 +9794,7 @@
         <v>23.594267640269699</v>
       </c>
     </row>
-    <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>44166</v>
       </c>
@@ -9800,7 +9811,7 @@
         <v>23.982140173238701</v>
       </c>
     </row>
-    <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>44167</v>
       </c>
@@ -9817,7 +9828,7 @@
         <v>24.340176357517699</v>
       </c>
     </row>
-    <row r="60" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>44168</v>
       </c>
@@ -9834,7 +9845,7 @@
         <v>24.397524195136398</v>
       </c>
     </row>
-    <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>44169</v>
       </c>
@@ -9851,7 +9862,7 @@
         <v>24.955158307730301</v>
       </c>
     </row>
-    <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>44172</v>
       </c>
@@ -9868,7 +9879,7 @@
         <v>24.781501050410601</v>
       </c>
     </row>
-    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>44173</v>
       </c>
@@ -9885,7 +9896,7 @@
         <v>24.752910752365899</v>
       </c>
     </row>
-    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>44174</v>
       </c>
@@ -9902,7 +9913,7 @@
         <v>24.643335655610599</v>
       </c>
     </row>
-    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>44175</v>
       </c>
@@ -9919,7 +9930,7 @@
         <v>24.270118954488201</v>
       </c>
     </row>
-    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>44176</v>
       </c>
@@ -9936,7 +9947,7 @@
         <v>23.436014531250301</v>
       </c>
     </row>
-    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>44179</v>
       </c>
@@ -9953,7 +9964,7 @@
         <v>23.0793985806623</v>
       </c>
     </row>
-    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>44180</v>
       </c>
@@ -9970,7 +9981,7 @@
         <v>23.1736417652676</v>
       </c>
     </row>
-    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>44181</v>
       </c>
@@ -9987,7 +9998,7 @@
         <v>23.576845978501499</v>
       </c>
     </row>
-    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>44182</v>
       </c>
@@ -10004,7 +10015,7 @@
         <v>24.234501542984301</v>
       </c>
     </row>
-    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>44183</v>
       </c>
@@ -10021,7 +10032,7 @@
         <v>24.143570230895801</v>
       </c>
     </row>
-    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>44186</v>
       </c>
@@ -10038,7 +10049,7 @@
         <v>24.930713863865499</v>
       </c>
     </row>
-    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>44187</v>
       </c>
@@ -10055,7 +10066,7 @@
         <v>26.010586205597001</v>
       </c>
     </row>
-    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>44188</v>
       </c>
@@ -10072,7 +10083,7 @@
         <v>25.8556520022392</v>
       </c>
     </row>
-    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>44189</v>
       </c>
@@ -10089,7 +10100,7 @@
         <v>25.684315353734402</v>
       </c>
     </row>
-    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>44193</v>
       </c>
@@ -10106,7 +10117,7 @@
         <v>25.3023353212877</v>
       </c>
     </row>
-    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>44194</v>
       </c>
@@ -10123,7 +10134,7 @@
         <v>25.228548361483998</v>
       </c>
     </row>
-    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>44195</v>
       </c>
@@ -10140,7 +10151,7 @@
         <v>24.867410295046501</v>
       </c>
     </row>
-    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>44196</v>
       </c>
@@ -10157,7 +10168,7 @@
         <v>25.231553005107699</v>
       </c>
     </row>
-    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>44200</v>
       </c>
@@ -10174,7 +10185,7 @@
         <v>25.867901677805801</v>
       </c>
     </row>
-    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>44201</v>
       </c>
@@ -10191,7 +10202,7 @@
         <v>26.568882046055801</v>
       </c>
     </row>
-    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>44202</v>
       </c>
@@ -10208,7 +10219,7 @@
         <v>27.210866999448701</v>
       </c>
     </row>
-    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>44203</v>
       </c>
@@ -10225,7 +10236,7 @@
         <v>27.219428674237601</v>
       </c>
     </row>
-    <row r="84" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>44204</v>
       </c>
@@ -10242,7 +10253,7 @@
         <v>27.779482870222399</v>
       </c>
     </row>
-    <row r="85" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>44207</v>
       </c>
@@ -10259,7 +10270,7 @@
         <v>28.285195451992902</v>
       </c>
     </row>
-    <row r="86" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>44208</v>
       </c>
@@ -10276,7 +10287,7 @@
         <v>28.776309354202599</v>
       </c>
     </row>
-    <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>44209</v>
       </c>
@@ -10293,7 +10304,7 @@
         <v>29.9467338099209</v>
       </c>
     </row>
-    <row r="88" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>44210</v>
       </c>
@@ -10310,7 +10321,7 @@
         <v>30.767575620766699</v>
       </c>
     </row>
-    <row r="89" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>44211</v>
       </c>
@@ -10327,7 +10338,7 @@
         <v>31.725237994305601</v>
       </c>
     </row>
-    <row r="90" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>44215</v>
       </c>
@@ -10344,7 +10355,7 @@
         <v>32.4126614797486</v>
       </c>
     </row>
-    <row r="91" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>44216</v>
       </c>
@@ -10361,7 +10372,7 @@
         <v>33.429619021126399</v>
       </c>
     </row>
-    <row r="92" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>44217</v>
       </c>
@@ -10378,7 +10389,7 @@
         <v>35.050508194038898</v>
       </c>
     </row>
-    <row r="93" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>44218</v>
       </c>
@@ -10395,7 +10406,7 @@
         <v>35.888247936616899</v>
       </c>
     </row>
-    <row r="94" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>44221</v>
       </c>
@@ -10412,7 +10423,7 @@
         <v>36.103342757609703</v>
       </c>
     </row>
-    <row r="95" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>44222</v>
       </c>
@@ -10429,7 +10440,7 @@
         <v>36.415849989486503</v>
       </c>
     </row>
-    <row r="96" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>44223</v>
       </c>
@@ -10446,7 +10457,7 @@
         <v>36.212543884613403</v>
       </c>
     </row>
-    <row r="97" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>44224</v>
       </c>
@@ -10463,7 +10474,7 @@
         <v>36.421114651918103</v>
       </c>
     </row>
-    <row r="98" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>44225</v>
       </c>
@@ -10480,7 +10491,7 @@
         <v>36.960353680080601</v>
       </c>
     </row>
-    <row r="99" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>44228</v>
       </c>
@@ -10497,7 +10508,7 @@
         <v>38.240121477322504</v>
       </c>
     </row>
-    <row r="100" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>44229</v>
       </c>
@@ -10514,7 +10525,7 @@
         <v>39.563628831842202</v>
       </c>
     </row>
-    <row r="101" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>44230</v>
       </c>
@@ -10531,7 +10542,7 @@
         <v>40.629711540836396</v>
       </c>
     </row>
-    <row r="102" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>44231</v>
       </c>
@@ -10548,7 +10559,7 @@
         <v>41.509881348053398</v>
       </c>
     </row>
-    <row r="103" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>44232</v>
       </c>
@@ -10565,7 +10576,7 @@
         <v>42.5133512658673</v>
       </c>
     </row>
-    <row r="104" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>44235</v>
       </c>
@@ -10582,7 +10593,7 @@
         <v>43.745551766263702</v>
       </c>
     </row>
-    <row r="105" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>44236</v>
       </c>
@@ -10599,7 +10610,7 @@
         <v>44.276567814340197</v>
       </c>
     </row>
-    <row r="106" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>44237</v>
       </c>
@@ -10616,7 +10627,7 @@
         <v>43.923694277576601</v>
       </c>
     </row>
-    <row r="107" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>44238</v>
       </c>
@@ -10633,7 +10644,7 @@
         <v>43.896680762728998</v>
       </c>
     </row>
-    <row r="108" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>44239</v>
       </c>
@@ -10650,7 +10661,7 @@
         <v>43.633845758115498</v>
       </c>
     </row>
-    <row r="109" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>44243</v>
       </c>
@@ -10667,7 +10678,7 @@
         <v>43.8500335984873</v>
       </c>
     </row>
-    <row r="110" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>44244</v>
       </c>
@@ -10684,7 +10695,7 @@
         <v>43.782047424802997</v>
       </c>
     </row>
-    <row r="111" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>44245</v>
       </c>
@@ -10701,7 +10712,7 @@
         <v>43.450508408196299</v>
       </c>
     </row>
-    <row r="112" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>44246</v>
       </c>
@@ -10718,7 +10729,7 @@
         <v>43.532396530303203</v>
       </c>
     </row>
-    <row r="113" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>44249</v>
       </c>
@@ -10735,7 +10746,7 @@
         <v>43.026802895908801</v>
       </c>
     </row>
-    <row r="114" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>44250</v>
       </c>
@@ -10752,7 +10763,7 @@
         <v>42.027460912437398</v>
       </c>
     </row>
-    <row r="115" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>44251</v>
       </c>
@@ -10769,7 +10780,7 @@
         <v>41.627002122888797</v>
       </c>
     </row>
-    <row r="116" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>44252</v>
       </c>
@@ -10786,7 +10797,7 @@
         <v>41.238349612574297</v>
       </c>
     </row>
-    <row r="117" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>44253</v>
       </c>
@@ -10803,7 +10814,7 @@
         <v>40.705264157696803</v>
       </c>
     </row>
-    <row r="118" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>44256</v>
       </c>
@@ -10820,7 +10831,7 @@
         <v>40.557244858385801</v>
       </c>
     </row>
-    <row r="119" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>44257</v>
       </c>
@@ -10837,7 +10848,7 @@
         <v>40.4843163828508</v>
       </c>
     </row>
-    <row r="120" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>44258</v>
       </c>
@@ -10854,7 +10865,7 @@
         <v>40.0915886764936</v>
       </c>
     </row>
-    <row r="121" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>44259</v>
       </c>
@@ -10871,7 +10882,7 @@
         <v>39.323319667903199</v>
       </c>
     </row>
-    <row r="122" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>44260</v>
       </c>
@@ -10888,7 +10899,7 @@
         <v>38.490709122037899</v>
       </c>
     </row>
-    <row r="123" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>44263</v>
       </c>
@@ -10905,7 +10916,7 @@
         <v>37.5657233075002</v>
       </c>
     </row>
-    <row r="124" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>44264</v>
       </c>
@@ -10922,7 +10933,7 @@
         <v>37.347224998984302</v>
       </c>
     </row>
-    <row r="125" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>44265</v>
       </c>
@@ -10939,7 +10950,7 @@
         <v>36.782143268420398</v>
       </c>
     </row>
-    <row r="126" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>44266</v>
       </c>
@@ -10956,7 +10967,7 @@
         <v>35.635223184054098</v>
       </c>
     </row>
-    <row r="127" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>44267</v>
       </c>
@@ -10973,7 +10984,7 @@
         <v>34.942166140387101</v>
       </c>
     </row>
-    <row r="128" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
         <v>44270</v>
       </c>
@@ -10990,7 +11001,7 @@
         <v>34.511935634854801</v>
       </c>
     </row>
-    <row r="129" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
         <v>44271</v>
       </c>
@@ -11007,7 +11018,7 @@
         <v>34.352298856028902</v>
       </c>
     </row>
-    <row r="130" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <v>44272</v>
       </c>
@@ -11024,7 +11035,7 @@
         <v>34.639682241563499</v>
       </c>
     </row>
-    <row r="131" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <v>44273</v>
       </c>
@@ -11041,7 +11052,7 @@
         <v>34.639159739029402</v>
       </c>
     </row>
-    <row r="132" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
         <v>44274</v>
       </c>
@@ -11058,7 +11069,7 @@
         <v>33.707922061204698</v>
       </c>
     </row>
-    <row r="133" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
         <v>44277</v>
       </c>
@@ -11075,7 +11086,7 @@
         <v>32.716381850179197</v>
       </c>
     </row>
-    <row r="134" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
         <v>44278</v>
       </c>
@@ -11092,7 +11103,7 @@
         <v>31.311982054147499</v>
       </c>
     </row>
-    <row r="135" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
         <v>44279</v>
       </c>
@@ -11109,7 +11120,7 @@
         <v>30.497549254426001</v>
       </c>
     </row>
-    <row r="136" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" s="1">
         <v>44280</v>
       </c>
@@ -11126,7 +11137,7 @@
         <v>29.718590066820401</v>
       </c>
     </row>
-    <row r="137" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
         <v>44281</v>
       </c>
@@ -11143,7 +11154,7 @@
         <v>29.775728571645999</v>
       </c>
     </row>
-    <row r="138" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" s="1">
         <v>44284</v>
       </c>
@@ -11160,7 +11171,7 @@
         <v>29.8580604377909</v>
       </c>
     </row>
-    <row r="139" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" s="1">
         <v>44285</v>
       </c>
@@ -11177,7 +11188,7 @@
         <v>29.678101497973699</v>
       </c>
     </row>
-    <row r="140" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" s="1">
         <v>44286</v>
       </c>
@@ -11194,7 +11205,7 @@
         <v>29.772524475077802</v>
       </c>
     </row>
-    <row r="141" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141" s="1">
         <v>44287</v>
       </c>
@@ -11211,7 +11222,7 @@
         <v>30.377567334614401</v>
       </c>
     </row>
-    <row r="142" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142" s="1">
         <v>44291</v>
       </c>
@@ -11228,7 +11239,7 @@
         <v>31.4124122418553</v>
       </c>
     </row>
-    <row r="143" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
         <v>44292</v>
       </c>
@@ -11245,7 +11256,7 @@
         <v>32.336865400770499</v>
       </c>
     </row>
-    <row r="144" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
         <v>44293</v>
       </c>
@@ -11262,7 +11273,7 @@
         <v>32.821301814369598</v>
       </c>
     </row>
-    <row r="145" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" s="1">
         <v>44294</v>
       </c>
@@ -11279,7 +11290,7 @@
         <v>33.735987273730601</v>
       </c>
     </row>
-    <row r="146" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146" s="1">
         <v>44295</v>
       </c>
@@ -11296,7 +11307,7 @@
         <v>34.146598538911697</v>
       </c>
     </row>
-    <row r="147" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147" s="1">
         <v>44298</v>
       </c>
@@ -11313,7 +11324,7 @@
         <v>33.898618576592597</v>
       </c>
     </row>
-    <row r="148" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148" s="1">
         <v>44299</v>
       </c>
@@ -11330,7 +11341,7 @@
         <v>33.035585488849698</v>
       </c>
     </row>
-    <row r="149" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149" s="1">
         <v>44300</v>
       </c>
@@ -11347,7 +11358,7 @@
         <v>32.628620034941697</v>
       </c>
     </row>
-    <row r="150" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150" s="1">
         <v>44301</v>
       </c>
@@ -11364,7 +11375,7 @@
         <v>32.210544571693198</v>
       </c>
     </row>
-    <row r="151" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A151" s="1">
         <v>44302</v>
       </c>
@@ -11381,7 +11392,7 @@
         <v>31.7301397004065</v>
       </c>
     </row>
-    <row r="152" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152" s="1">
         <v>44305</v>
       </c>
@@ -11398,7 +11409,7 @@
         <v>30.734721037219899</v>
       </c>
     </row>
-    <row r="153" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153" s="1">
         <v>44306</v>
       </c>
@@ -11415,7 +11426,7 @@
         <v>29.889275212546998</v>
       </c>
     </row>
-    <row r="154" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154" s="1">
         <v>44307</v>
       </c>
@@ -11432,7 +11443,7 @@
         <v>29.5151822604426</v>
       </c>
     </row>
-    <row r="155" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155" s="1">
         <v>44308</v>
       </c>
@@ -11449,7 +11460,7 @@
         <v>29.110551542395299</v>
       </c>
     </row>
-    <row r="156" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156" s="1">
         <v>44309</v>
       </c>
@@ -11466,7 +11477,7 @@
         <v>30.020290019135199</v>
       </c>
     </row>
-    <row r="157" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157" s="1">
         <v>44312</v>
       </c>
@@ -11483,7 +11494,7 @@
         <v>31.0024407687871</v>
       </c>
     </row>
-    <row r="158" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A158" s="1">
         <v>44313</v>
       </c>
@@ -11500,7 +11511,7 @@
         <v>32.255397741501902</v>
       </c>
     </row>
-    <row r="159" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A159" s="1">
         <v>44314</v>
       </c>
@@ -11517,7 +11528,7 @@
         <v>32.578973543255501</v>
       </c>
     </row>
-    <row r="160" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A160" s="1">
         <v>44315</v>
       </c>
@@ -11534,7 +11545,7 @@
         <v>32.587013007347799</v>
       </c>
     </row>
-    <row r="161" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A161" s="1">
         <v>44316</v>
       </c>
@@ -11551,7 +11562,7 @@
         <v>32.522731907851103</v>
       </c>
     </row>
-    <row r="162" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A162" s="1">
         <v>44319</v>
       </c>
@@ -11568,7 +11579,7 @@
         <v>32.443577288215003</v>
       </c>
     </row>
-    <row r="163" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163" s="1">
         <v>44320</v>
       </c>
@@ -11585,7 +11596,7 @@
         <v>32.688904564029102</v>
       </c>
     </row>
-    <row r="164" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A164" s="1">
         <v>44321</v>
       </c>
@@ -11602,7 +11613,7 @@
         <v>32.06001148376</v>
       </c>
     </row>
-    <row r="165" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A165" s="1">
         <v>44322</v>
       </c>
@@ -11619,7 +11630,7 @@
         <v>31.277463569972401</v>
       </c>
     </row>
-    <row r="166" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A166" s="1">
         <v>44323</v>
       </c>
@@ -11636,7 +11647,7 @@
         <v>30.143191159125301</v>
       </c>
     </row>
-    <row r="167" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A167" s="1">
         <v>44326</v>
       </c>
@@ -11653,7 +11664,7 @@
         <v>29.419634486437602</v>
       </c>
     </row>
-    <row r="168" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A168" s="1">
         <v>44327</v>
       </c>
@@ -11670,7 +11681,7 @@
         <v>30.3877889421126</v>
       </c>
     </row>
-    <row r="169" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A169" s="1">
         <v>44328</v>
       </c>
@@ -11687,7 +11698,7 @@
         <v>31.446954123479401</v>
       </c>
     </row>
-    <row r="170" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A170" s="1">
         <v>44329</v>
       </c>
@@ -11704,7 +11715,7 @@
         <v>32.571478179290999</v>
       </c>
     </row>
-    <row r="171" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A171" s="1">
         <v>44330</v>
       </c>
@@ -11721,7 +11732,7 @@
         <v>32.923844986517899</v>
       </c>
     </row>
-    <row r="172" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A172" s="1">
         <v>44333</v>
       </c>
@@ -11738,7 +11749,7 @@
         <v>33.1528684827693</v>
       </c>
     </row>
-    <row r="173" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173" s="1">
         <v>44334</v>
       </c>
@@ -11755,7 +11766,7 @@
         <v>33.3170157531911</v>
       </c>
     </row>
-    <row r="174" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A174" s="1">
         <v>44335</v>
       </c>
@@ -11772,7 +11783,7 @@
         <v>33.804275117512503</v>
       </c>
     </row>
-    <row r="175" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A175" s="1">
         <v>44336</v>
       </c>
@@ -11789,7 +11800,7 @@
         <v>34.037243538758602</v>
       </c>
     </row>
-    <row r="176" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176" s="1">
         <v>44337</v>
       </c>
@@ -11806,7 +11817,7 @@
         <v>33.817582845618702</v>
       </c>
     </row>
-    <row r="177" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A177" s="1">
         <v>44340</v>
       </c>
@@ -11823,7 +11834,7 @@
         <v>33.098074500363403</v>
       </c>
     </row>
-    <row r="178" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A178" s="1">
         <v>44341</v>
       </c>
@@ -11840,7 +11851,7 @@
         <v>31.897921410269401</v>
       </c>
     </row>
-    <row r="179" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A179" s="1">
         <v>44342</v>
       </c>
@@ -11857,7 +11868,7 @@
         <v>31.172865949766301</v>
       </c>
     </row>
-    <row r="180" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A180" s="1">
         <v>44343</v>
       </c>
@@ -11874,7 +11885,7 @@
         <v>30.713337550803601</v>
       </c>
     </row>
-    <row r="181" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A181" s="1">
         <v>44344</v>
       </c>
@@ -11891,7 +11902,7 @@
         <v>30.4228375646255</v>
       </c>
     </row>
-    <row r="182" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A182" s="1">
         <v>44348</v>
       </c>
@@ -11908,7 +11919,7 @@
         <v>30.2202522049027</v>
       </c>
     </row>
-    <row r="183" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A183" s="1">
         <v>44349</v>
       </c>
@@ -11925,7 +11936,7 @@
         <v>29.220612815684799</v>
       </c>
     </row>
-    <row r="184" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A184" s="1">
         <v>44350</v>
       </c>
@@ -11942,7 +11953,7 @@
         <v>28.637637929247401</v>
       </c>
     </row>
-    <row r="185" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A185" s="1">
         <v>44351</v>
       </c>
@@ -11959,7 +11970,7 @@
         <v>27.560889416346999</v>
       </c>
     </row>
-    <row r="186" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A186" s="1">
         <v>44354</v>
       </c>
@@ -11976,7 +11987,7 @@
         <v>26.850521064063098</v>
       </c>
     </row>
-    <row r="187" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A187" s="1">
         <v>44355</v>
       </c>
@@ -11993,7 +12004,7 @@
         <v>25.712131145003301</v>
       </c>
     </row>
-    <row r="188" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A188" s="1">
         <v>44356</v>
       </c>
@@ -12010,7 +12021,7 @@
         <v>24.421934390281798</v>
       </c>
     </row>
-    <row r="189" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A189" s="1">
         <v>44357</v>
       </c>
@@ -12027,7 +12038,7 @@
         <v>23.2637369117862</v>
       </c>
     </row>
-    <row r="190" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A190" s="1">
         <v>44358</v>
       </c>
@@ -12044,7 +12055,7 @@
         <v>22.113537972352798</v>
       </c>
     </row>
-    <row r="191" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A191" s="1">
         <v>44361</v>
       </c>
@@ -12061,7 +12072,7 @@
         <v>21.2231813840441</v>
       </c>
     </row>
-    <row r="192" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A192" s="1">
         <v>44362</v>
       </c>
@@ -12078,7 +12089,7 @@
         <v>20.397751411880598</v>
       </c>
     </row>
-    <row r="193" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A193" s="1">
         <v>44363</v>
       </c>
@@ -12095,7 +12106,7 @@
         <v>19.0067748956345</v>
       </c>
     </row>
-    <row r="194" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A194" s="1">
         <v>44364</v>
       </c>
@@ -12112,7 +12123,7 @@
         <v>17.834739208473898</v>
       </c>
     </row>
-    <row r="195" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A195" s="1">
         <v>44365</v>
       </c>
@@ -12129,7 +12140,7 @@
         <v>17.6605735109104</v>
       </c>
     </row>
-    <row r="196" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A196" s="1">
         <v>44368</v>
       </c>
@@ -12146,7 +12157,7 @@
         <v>17.862526215176601</v>
       </c>
     </row>
-    <row r="197" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A197" s="1">
         <v>44369</v>
       </c>
@@ -12163,7 +12174,7 @@
         <v>17.441935951406599</v>
       </c>
     </row>
-    <row r="198" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A198" s="1">
         <v>44370</v>
       </c>
@@ -12180,7 +12191,7 @@
         <v>17.200325547030999</v>
       </c>
     </row>
-    <row r="199" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A199" s="1">
         <v>44371</v>
       </c>
@@ -12197,7 +12208,7 @@
         <v>16.815940905665499</v>
       </c>
     </row>
-    <row r="200" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A200" s="1">
         <v>44372</v>
       </c>
@@ -12214,7 +12225,7 @@
         <v>16.182940534317598</v>
       </c>
     </row>
-    <row r="201" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A201" s="1">
         <v>44375</v>
       </c>
@@ -12231,7 +12242,7 @@
         <v>15.685757734041999</v>
       </c>
     </row>
-    <row r="202" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A202" s="1">
         <v>44376</v>
       </c>
@@ -12248,7 +12259,7 @@
         <v>14.9111153131726</v>
       </c>
     </row>
-    <row r="203" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A203" s="1">
         <v>44377</v>
       </c>
@@ -12265,7 +12276,7 @@
         <v>14.620895284998401</v>
       </c>
     </row>
-    <row r="204" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A204" s="1">
         <v>44378</v>
       </c>
@@ -12282,7 +12293,7 @@
         <v>14.3080539022362</v>
       </c>
     </row>
-    <row r="205" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A205" s="1">
         <v>44379</v>
       </c>
@@ -12299,7 +12310,7 @@
         <v>13.4655822567002</v>
       </c>
     </row>
-    <row r="206" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A206" s="1">
         <v>44383</v>
       </c>
@@ -12316,7 +12327,7 @@
         <v>12.8659609900392</v>
       </c>
     </row>
-    <row r="207" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A207" s="1">
         <v>44384</v>
       </c>
@@ -12333,7 +12344,7 @@
         <v>13.2201778344754</v>
       </c>
     </row>
-    <row r="208" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A208" s="1">
         <v>44385</v>
       </c>
@@ -12350,7 +12361,7 @@
         <v>14.0905498696865</v>
       </c>
     </row>
-    <row r="209" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A209" s="1">
         <v>44386</v>
       </c>
@@ -12367,7 +12378,7 @@
         <v>14.3874537760402</v>
       </c>
     </row>
-    <row r="210" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A210" s="1">
         <v>44389</v>
       </c>
@@ -12384,7 +12395,7 @@
         <v>14.345066584391899</v>
       </c>
     </row>
-    <row r="211" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A211" s="1">
         <v>44390</v>
       </c>
@@ -12401,7 +12412,7 @@
         <v>14.4305281927815</v>
       </c>
     </row>
-    <row r="212" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A212" s="1">
         <v>44391</v>
       </c>
@@ -12418,7 +12429,7 @@
         <v>14.324511883784099</v>
       </c>
     </row>
-    <row r="213" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A213" s="1">
         <v>44392</v>
       </c>
@@ -12435,7 +12446,7 @@
         <v>13.704226552673299</v>
       </c>
     </row>
-    <row r="214" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A214" s="1">
         <v>44393</v>
       </c>
@@ -12452,7 +12463,7 @@
         <v>13.204856865299099</v>
       </c>
     </row>
-    <row r="215" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A215" s="1">
         <v>44396</v>
       </c>
@@ -12469,7 +12480,7 @@
         <v>13.4488434804568</v>
       </c>
     </row>
-    <row r="216" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A216" s="1">
         <v>44397</v>
       </c>
@@ -12486,7 +12497,7 @@
         <v>12.973127513487301</v>
       </c>
     </row>
-    <row r="217" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A217" s="1">
         <v>44398</v>
       </c>
@@ -12503,7 +12514,7 @@
         <v>12.1485373675504</v>
       </c>
     </row>
-    <row r="218" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A218" s="1">
         <v>44399</v>
       </c>
@@ -12520,7 +12531,7 @@
         <v>11.5989526290242</v>
       </c>
     </row>
-    <row r="219" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A219" s="1">
         <v>44400</v>
       </c>
@@ -12537,7 +12548,7 @@
         <v>12.2291549007381</v>
       </c>
     </row>
-    <row r="220" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A220" s="1">
         <v>44403</v>
       </c>
@@ -12554,7 +12565,7 @@
         <v>13.354282714974801</v>
       </c>
     </row>
-    <row r="221" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A221" s="1">
         <v>44404</v>
       </c>
@@ -12571,7 +12582,7 @@
         <v>14.223864165837201</v>
       </c>
     </row>
-    <row r="222" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A222" s="1">
         <v>44405</v>
       </c>
@@ -12588,7 +12599,7 @@
         <v>14.136094349596499</v>
       </c>
     </row>
-    <row r="223" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A223" s="1">
         <v>44406</v>
       </c>
@@ -12605,7 +12616,7 @@
         <v>14.1916811859364</v>
       </c>
     </row>
-    <row r="224" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A224" s="1">
         <v>44407</v>
       </c>
@@ -12622,7 +12633,7 @@
         <v>14.3633137751406</v>
       </c>
     </row>
-    <row r="225" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A225" s="1">
         <v>44410</v>
       </c>
@@ -12639,7 +12650,7 @@
         <v>13.926005154219601</v>
       </c>
     </row>
-    <row r="226" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A226" s="1">
         <v>44411</v>
       </c>
@@ -12656,7 +12667,7 @@
         <v>14.0343362953903</v>
       </c>
     </row>
-    <row r="227" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A227" s="1">
         <v>44412</v>
       </c>
@@ -12673,7 +12684,7 @@
         <v>14.407524942576799</v>
       </c>
     </row>
-    <row r="228" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A228" s="1">
         <v>44413</v>
       </c>
@@ -12690,7 +12701,7 @@
         <v>14.2355116129969</v>
       </c>
     </row>
-    <row r="229" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A229" s="1">
         <v>44414</v>
       </c>
@@ -12707,7 +12718,7 @@
         <v>13.569153237667001</v>
       </c>
     </row>
-    <row r="230" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A230" s="1">
         <v>44417</v>
       </c>
@@ -12724,7 +12735,7 @@
         <v>12.835409186686601</v>
       </c>
     </row>
-    <row r="231" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A231" s="1">
         <v>44418</v>
       </c>
@@ -12741,7 +12752,7 @@
         <v>13.4968352371045</v>
       </c>
     </row>
-    <row r="232" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A232" s="1">
         <v>44419</v>
       </c>
@@ -12758,7 +12769,7 @@
         <v>14.1073823605672</v>
       </c>
     </row>
-    <row r="233" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A233" s="1">
         <v>44420</v>
       </c>
@@ -12775,7 +12786,7 @@
         <v>15.169326001510001</v>
       </c>
     </row>
-    <row r="234" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A234" s="1">
         <v>44421</v>
       </c>
@@ -12792,7 +12803,7 @@
         <v>15.8374359394625</v>
       </c>
     </row>
-    <row r="235" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A235" s="1">
         <v>44424</v>
       </c>
@@ -12809,7 +12820,7 @@
         <v>16.383859374786699</v>
       </c>
     </row>
-    <row r="236" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A236" s="1">
         <v>44425</v>
       </c>
@@ -12826,7 +12837,7 @@
         <v>17.342927058517098</v>
       </c>
     </row>
-    <row r="237" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A237" s="1">
         <v>44426</v>
       </c>
@@ -12843,7 +12854,7 @@
         <v>17.933572646149901</v>
       </c>
     </row>
-    <row r="238" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A238" s="1">
         <v>44427</v>
       </c>
@@ -12860,7 +12871,7 @@
         <v>18.852010031002099</v>
       </c>
     </row>
-    <row r="239" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A239" s="1">
         <v>44428</v>
       </c>
@@ -12877,7 +12888,7 @@
         <v>19.5924626307939</v>
       </c>
     </row>
-    <row r="240" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A240" s="1">
         <v>44431</v>
       </c>
@@ -12894,7 +12905,7 @@
         <v>19.154287577030299</v>
       </c>
     </row>
-    <row r="241" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A241" s="1">
         <v>44432</v>
       </c>
@@ -12911,7 +12922,7 @@
         <v>18.333114272717498</v>
       </c>
     </row>
-    <row r="242" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A242" s="1">
         <v>44433</v>
       </c>
@@ -12928,7 +12939,7 @@
         <v>17.183462802527899</v>
       </c>
     </row>
-    <row r="243" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A243" s="1">
         <v>44434</v>
       </c>
@@ -12945,7 +12956,7 @@
         <v>16.812203175238899</v>
       </c>
     </row>
-    <row r="244" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A244" s="1">
         <v>44435</v>
       </c>
@@ -12962,7 +12973,7 @@
         <v>16.316567908276902</v>
       </c>
     </row>
-    <row r="245" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A245" s="1">
         <v>44438</v>
       </c>
@@ -12979,7 +12990,7 @@
         <v>16.071926575438301</v>
       </c>
     </row>
-    <row r="246" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A246" s="1">
         <v>44439</v>
       </c>
@@ -12996,7 +13007,7 @@
         <v>15.8899538052958</v>
       </c>
     </row>
-    <row r="247" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A247" s="1">
         <v>44440</v>
       </c>
@@ -13013,7 +13024,7 @@
         <v>15.6595134154998</v>
       </c>
     </row>
-    <row r="248" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A248" s="1">
         <v>44441</v>
       </c>
@@ -13030,7 +13041,7 @@
         <v>15.851781803602501</v>
       </c>
     </row>
-    <row r="249" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A249" s="1">
         <v>44442</v>
       </c>
@@ -13047,7 +13058,7 @@
         <v>16.1206477496745</v>
       </c>
     </row>
-    <row r="250" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A250" s="1">
         <v>44446</v>
       </c>
@@ -13064,7 +13075,7 @@
         <v>16.618962974561899</v>
       </c>
     </row>
-    <row r="251" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A251" s="1">
         <v>44447</v>
       </c>
@@ -13081,7 +13092,7 @@
         <v>17.341229968852801</v>
       </c>
     </row>
-    <row r="252" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A252" s="1">
         <v>44448</v>
       </c>
@@ -13098,7 +13109,7 @@
         <v>16.886268202319101</v>
       </c>
     </row>
-    <row r="253" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A253" s="1">
         <v>44449</v>
       </c>
@@ -13115,7 +13126,7 @@
         <v>16.442797625721301</v>
       </c>
     </row>
-    <row r="254" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A254" s="1">
         <v>44452</v>
       </c>
@@ -13132,7 +13143,7 @@
         <v>16.155296729086199</v>
       </c>
     </row>
-    <row r="255" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A255" s="1">
         <v>44453</v>
       </c>
@@ -13149,7 +13160,7 @@
         <v>16.2457875905789</v>
       </c>
     </row>
-    <row r="256" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A256" s="1">
         <v>44454</v>
       </c>
@@ -13166,7 +13177,7 @@
         <v>16.176383544030699</v>
       </c>
     </row>
-    <row r="257" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A257" s="1">
         <v>44455</v>
       </c>
@@ -13183,7 +13194,7 @@
         <v>15.771497824798599</v>
       </c>
     </row>
-    <row r="258" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A258" s="1">
         <v>44456</v>
       </c>
@@ -13200,7 +13211,7 @@
         <v>14.774338774677201</v>
       </c>
     </row>
-    <row r="259" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A259" s="1">
         <v>44459</v>
       </c>
@@ -13217,7 +13228,7 @@
         <v>14.6056332361449</v>
       </c>
     </row>
-    <row r="260" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A260" s="1">
         <v>44460</v>
       </c>
@@ -13234,7 +13245,7 @@
         <v>14.4272526519891</v>
       </c>
     </row>
-    <row r="261" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A261" s="1">
         <v>44461</v>
       </c>
@@ -13251,7 +13262,7 @@
         <v>13.917481128174</v>
       </c>
     </row>
-    <row r="262" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A262" s="1">
         <v>44462</v>
       </c>
@@ -13268,7 +13279,7 @@
         <v>13.0906434802751</v>
       </c>
     </row>
-    <row r="263" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A263" s="1">
         <v>44463</v>
       </c>
@@ -13285,7 +13296,7 @@
         <v>12.4197635811336</v>
       </c>
     </row>
-    <row r="264" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A264" s="1">
         <v>44466</v>
       </c>
@@ -13302,7 +13313,7 @@
         <v>12.0453921190685</v>
       </c>
     </row>
-    <row r="265" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A265" s="1">
         <v>44467</v>
       </c>
@@ -13319,7 +13330,7 @@
         <v>12.0144495930655</v>
       </c>
     </row>
-    <row r="266" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A266" s="1">
         <v>44468</v>
       </c>
@@ -13336,7 +13347,7 @@
         <v>12.3465104869614</v>
       </c>
     </row>
-    <row r="267" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A267" s="1">
         <v>44469</v>
       </c>
@@ -13353,7 +13364,7 @@
         <v>12.5201644154895</v>
       </c>
     </row>
-    <row r="268" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A268" s="1">
         <v>44470</v>
       </c>
@@ -13370,7 +13381,7 @@
         <v>12.8422824760846</v>
       </c>
     </row>
-    <row r="269" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A269" s="1">
         <v>44473</v>
       </c>
@@ -13387,7 +13398,7 @@
         <v>12.7284912374152</v>
       </c>
     </row>
-    <row r="270" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A270" s="1">
         <v>44474</v>
       </c>
@@ -13404,7 +13415,7 @@
         <v>12.0610448126113</v>
       </c>
     </row>
-    <row r="271" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A271" s="1">
         <v>44475</v>
       </c>
@@ -13421,7 +13432,7 @@
         <v>12.640981555167601</v>
       </c>
     </row>
-    <row r="272" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A272" s="1">
         <v>44476</v>
       </c>
@@ -13438,7 +13449,7 @@
         <v>12.797230215613199</v>
       </c>
     </row>
-    <row r="273" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A273" s="1">
         <v>44477</v>
       </c>
@@ -13455,7 +13466,7 @@
         <v>12.436794319932201</v>
       </c>
     </row>
-    <row r="274" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A274" s="1">
         <v>44480</v>
       </c>
@@ -13472,7 +13483,7 @@
         <v>11.969233346332301</v>
       </c>
     </row>
-    <row r="275" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A275" s="1">
         <v>44481</v>
       </c>
@@ -13489,7 +13500,7 @@
         <v>12.295927747814799</v>
       </c>
     </row>
-    <row r="276" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A276" s="1">
         <v>44482</v>
       </c>
@@ -13506,7 +13517,7 @@
         <v>12.9127945271409</v>
       </c>
     </row>
-    <row r="277" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A277" s="1">
         <v>44483</v>
       </c>
@@ -13523,7 +13534,7 @@
         <v>12.357995322819299</v>
       </c>
     </row>
-    <row r="278" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A278" s="1">
         <v>44484</v>
       </c>
@@ -13540,7 +13551,7 @@
         <v>11.9094529241013</v>
       </c>
     </row>
-    <row r="279" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A279" s="1">
         <v>44487</v>
       </c>
@@ -13557,7 +13568,7 @@
         <v>11.4365504337731</v>
       </c>
     </row>
-    <row r="280" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A280" s="1">
         <v>44488</v>
       </c>
@@ -13574,7 +13585,7 @@
         <v>11.557771346795899</v>
       </c>
     </row>
-    <row r="281" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A281" s="1">
         <v>44489</v>
       </c>
@@ -13591,7 +13602,7 @@
         <v>11.594075535605</v>
       </c>
     </row>
-    <row r="282" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A282" s="1">
         <v>44490</v>
       </c>
@@ -13608,7 +13619,7 @@
         <v>11.9220897625404</v>
       </c>
     </row>
-    <row r="283" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A283" s="1">
         <v>44491</v>
       </c>
@@ -13625,7 +13636,7 @@
         <v>13.0740755525179</v>
       </c>
     </row>
-    <row r="284" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A284" s="1">
         <v>44494</v>
       </c>
@@ -13642,7 +13653,7 @@
         <v>13.7583694875063</v>
       </c>
     </row>
-    <row r="285" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A285" s="1">
         <v>44495</v>
       </c>
@@ -13659,7 +13670,7 @@
         <v>14.566230291065001</v>
       </c>
     </row>
-    <row r="286" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A286" s="1">
         <v>44496</v>
       </c>
@@ -13676,7 +13687,7 @@
         <v>15.545708922303101</v>
       </c>
     </row>
-    <row r="287" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A287" s="1">
         <v>44497</v>
       </c>
@@ -13693,7 +13704,7 @@
         <v>17.3071132278615</v>
       </c>
     </row>
-    <row r="288" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A288" s="1">
         <v>44498</v>
       </c>
@@ -13710,7 +13721,7 @@
         <v>18.470100927856699</v>
       </c>
     </row>
-    <row r="289" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A289" s="1">
         <v>44501</v>
       </c>
@@ -13727,7 +13738,7 @@
         <v>18.243918110207201</v>
       </c>
     </row>
-    <row r="290" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A290" s="1">
         <v>44502</v>
       </c>
@@ -13744,7 +13755,7 @@
         <v>17.890262022548001</v>
       </c>
     </row>
-    <row r="291" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A291" s="1">
         <v>44503</v>
       </c>
@@ -13761,7 +13772,7 @@
         <v>17.2025377861777</v>
       </c>
     </row>
-    <row r="292" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A292" s="1">
         <v>44504</v>
       </c>
@@ -13778,7 +13789,7 @@
         <v>16.830719970102599</v>
       </c>
     </row>
-    <row r="293" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A293" s="1">
         <v>44505</v>
       </c>
@@ -13795,7 +13806,7 @@
         <v>16.325510238159101</v>
       </c>
     </row>
-    <row r="294" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A294" s="1">
         <v>44508</v>
       </c>
@@ -13812,7 +13823,7 @@
         <v>16.3410075027871</v>
       </c>
     </row>
-    <row r="295" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A295" s="1">
         <v>44509</v>
       </c>
@@ -13829,7 +13840,7 @@
         <v>16.706122931370398</v>
       </c>
     </row>
-    <row r="296" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A296" s="1">
         <v>44510</v>
       </c>
@@ -13846,7 +13857,7 @@
         <v>17.014271758633502</v>
       </c>
     </row>
-    <row r="297" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A297" s="1">
         <v>44511</v>
       </c>
@@ -13863,7 +13874,7 @@
         <v>17.474285122894798</v>
       </c>
     </row>
-    <row r="298" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A298" s="1">
         <v>44512</v>
       </c>
@@ -13880,7 +13891,7 @@
         <v>18.037222738093099</v>
       </c>
     </row>
-    <row r="299" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A299" s="1">
         <v>44515</v>
       </c>
@@ -13897,7 +13908,7 @@
         <v>18.590844785002702</v>
       </c>
     </row>
-    <row r="300" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A300" s="1">
         <v>44516</v>
       </c>
@@ -13914,7 +13925,7 @@
         <v>18.528816054685699</v>
       </c>
     </row>
-    <row r="301" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A301" s="1">
         <v>44517</v>
       </c>
@@ -13931,7 +13942,7 @@
         <v>18.2397778806316</v>
       </c>
     </row>
-    <row r="302" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A302" s="1">
         <v>44518</v>
       </c>
@@ -13948,7 +13959,7 @@
         <v>18.359440895075899</v>
       </c>
     </row>
-    <row r="303" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A303" s="1">
         <v>44519</v>
       </c>
@@ -13965,7 +13976,7 @@
         <v>18.167489952158999</v>
       </c>
     </row>
-    <row r="304" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A304" s="1">
         <v>44522</v>
       </c>
@@ -13982,7 +13993,7 @@
         <v>17.306734892806801</v>
       </c>
     </row>
-    <row r="305" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A305" s="1">
         <v>44523</v>
       </c>
@@ -13999,7 +14010,7 @@
         <v>16.455825177932901</v>
       </c>
     </row>
-    <row r="306" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A306" s="1">
         <v>44524</v>
       </c>
@@ -14016,7 +14027,7 @@
         <v>15.8526622123298</v>
       </c>
     </row>
-    <row r="307" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A307" s="1">
         <v>44526</v>
       </c>
@@ -14033,7 +14044,7 @@
         <v>15.414701549950699</v>
       </c>
     </row>
-    <row r="308" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A308" s="1">
         <v>44529</v>
       </c>
@@ -14050,7 +14061,7 @@
         <v>14.3847359940396</v>
       </c>
     </row>
-    <row r="309" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A309" s="1">
         <v>44530</v>
       </c>
@@ -14067,7 +14078,7 @@
         <v>13.4374336639045</v>
       </c>
     </row>
-    <row r="310" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A310" s="1">
         <v>44531</v>
       </c>
@@ -14084,7 +14095,7 @@
         <v>12.5904413333816</v>
       </c>
     </row>
-    <row r="311" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A311" s="1">
         <v>44532</v>
       </c>
@@ -14101,7 +14112,7 @@
         <v>11.879927563626699</v>
       </c>
     </row>
-    <row r="312" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A312" s="1">
         <v>44533</v>
       </c>
@@ -14118,7 +14129,7 @@
         <v>11.2030485867047</v>
       </c>
     </row>
-    <row r="313" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A313" s="1">
         <v>44536</v>
       </c>
@@ -14135,7 +14146,7 @@
         <v>11.169165875368799</v>
       </c>
     </row>
-    <row r="314" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A314" s="1">
         <v>44537</v>
       </c>
@@ -14152,7 +14163,7 @@
         <v>12.870250967742701</v>
       </c>
     </row>
-    <row r="315" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A315" s="1">
         <v>44538</v>
       </c>
@@ -14169,7 +14180,7 @@
         <v>13.9632021833885</v>
       </c>
     </row>
-    <row r="316" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A316" s="1">
         <v>44539</v>
       </c>
@@ -14186,7 +14197,7 @@
         <v>13.9255461243193</v>
       </c>
     </row>
-    <row r="317" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A317" s="1">
         <v>44540</v>
       </c>
@@ -14203,7 +14214,7 @@
         <v>13.957026139876</v>
       </c>
     </row>
-    <row r="318" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A318" s="1">
         <v>44543</v>
       </c>
@@ -14220,7 +14231,7 @@
         <v>13.9406033580574</v>
       </c>
     </row>
-    <row r="319" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A319" s="1">
         <v>44544</v>
       </c>
@@ -14237,7 +14248,7 @@
         <v>13.8773038551253</v>
       </c>
     </row>
-    <row r="320" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A320" s="1">
         <v>44545</v>
       </c>
@@ -14254,7 +14265,7 @@
         <v>13.420178116472499</v>
       </c>
     </row>
-    <row r="321" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A321" s="1">
         <v>44546</v>
       </c>
@@ -14271,7 +14282,7 @@
         <v>13.3532403187226</v>
       </c>
     </row>
-    <row r="322" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A322" s="1">
         <v>44547</v>
       </c>
@@ -14288,7 +14299,7 @@
         <v>12.8894326093833</v>
       </c>
     </row>
-    <row r="323" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A323" s="1">
         <v>44550</v>
       </c>
@@ -14305,7 +14316,7 @@
         <v>11.9931648169967</v>
       </c>
     </row>
-    <row r="324" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A324" s="1">
         <v>44551</v>
       </c>
@@ -14322,7 +14333,7 @@
         <v>11.483675185519999</v>
       </c>
     </row>
-    <row r="325" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A325" s="1">
         <v>44552</v>
       </c>
@@ -14339,7 +14350,7 @@
         <v>11.7346363946004</v>
       </c>
     </row>
-    <row r="326" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A326" s="1">
         <v>44553</v>
       </c>
@@ -14356,7 +14367,7 @@
         <v>13.4340432406148</v>
       </c>
     </row>
-    <row r="327" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A327" s="1">
         <v>44557</v>
       </c>
@@ -14373,7 +14384,7 @@
         <v>14.651787637433401</v>
       </c>
     </row>
-    <row r="328" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A328" s="1">
         <v>44558</v>
       </c>
@@ -14390,7 +14401,7 @@
         <v>15.3036394985751</v>
       </c>
     </row>
-    <row r="329" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A329" s="1">
         <v>44559</v>
       </c>
@@ -14407,7 +14418,7 @@
         <v>15.727525146688</v>
       </c>
     </row>
-    <row r="330" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A330" s="1">
         <v>44560</v>
       </c>
@@ -14424,7 +14435,7 @@
         <v>16.061519808152401</v>
       </c>
     </row>
-    <row r="331" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A331" s="1">
         <v>44561</v>
       </c>
@@ -14441,7 +14452,7 @@
         <v>15.9105131228195</v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A332" s="1">
         <v>44564</v>
       </c>
@@ -14458,7 +14469,7 @@
         <v>16.462377377822101</v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A333" s="1">
         <v>44565</v>
       </c>
@@ -14475,7 +14486,7 @@
         <v>17.466908274506299</v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A334" s="1">
         <v>44566</v>
       </c>
@@ -14492,7 +14503,7 @@
         <v>18.705073902448898</v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A335" s="1">
         <v>44567</v>
       </c>
@@ -14509,7 +14520,7 @@
         <v>19.053209917591701</v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A336" s="1">
         <v>44568</v>
       </c>
@@ -14526,7 +14537,7 @@
         <v>19.489736926748702</v>
       </c>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A337" s="1">
         <v>44571</v>
       </c>
@@ -14543,7 +14554,7 @@
         <v>20.214359507657299</v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A338" s="1">
         <v>44572</v>
       </c>
@@ -14560,7 +14571,7 @@
         <v>21.3500704211176</v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A339" s="1">
         <v>44573</v>
       </c>
@@ -14577,7 +14588,7 @@
         <v>22.570189741410299</v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A340" s="1">
         <v>44574</v>
       </c>
@@ -14594,7 +14605,7 @@
         <v>23.688845047800299</v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A341" s="1">
         <v>44575</v>
       </c>
@@ -14611,7 +14622,7 @@
         <v>24.532946611109399</v>
       </c>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A342" s="1">
         <v>44579</v>
       </c>
@@ -14628,7 +14639,7 @@
         <v>25.3056397896673</v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A343" s="1">
         <v>44580</v>
       </c>
@@ -14645,7 +14656,7 @@
         <v>24.994172835483301</v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A344" s="1">
         <v>44581</v>
       </c>
@@ -14662,7 +14673,7 @@
         <v>24.260701580423401</v>
       </c>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A345" s="1">
         <v>44582</v>
       </c>
@@ -14679,7 +14690,7 @@
         <v>23.850257651789502</v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A346" s="1">
         <v>44585</v>
       </c>
@@ -14696,7 +14707,7 @@
         <v>24.939268494975799</v>
       </c>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A347" s="1">
         <v>44586</v>
       </c>
@@ -14713,7 +14724,7 @@
         <v>25.655198748879599</v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A348" s="1">
         <v>44587</v>
       </c>
@@ -14730,7 +14741,7 @@
         <v>25.547966433289101</v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A349" s="1">
         <v>44588</v>
       </c>
@@ -14747,7 +14758,7 @@
         <v>26.645691238928102</v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A350" s="1">
         <v>44589</v>
       </c>
@@ -14764,7 +14775,7 @@
         <v>28.169908826291199</v>
       </c>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A351" s="1">
         <v>44592</v>
       </c>
@@ -14781,7 +14792,7 @@
         <v>29.3084381062415</v>
       </c>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A352" s="1">
         <v>44593</v>
       </c>
@@ -14798,7 +14809,7 @@
         <v>30.253552950987299</v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A353" s="1">
         <v>44594</v>
       </c>
@@ -14815,7 +14826,7 @@
         <v>30.666705538384001</v>
       </c>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A354" s="1">
         <v>44595</v>
       </c>
@@ -14832,7 +14843,7 @@
         <v>30.997507388966401</v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A355" s="1">
         <v>44596</v>
       </c>
@@ -14849,7 +14860,7 @@
         <v>30.651489010647701</v>
       </c>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A356" s="1">
         <v>44599</v>
       </c>
@@ -14866,7 +14877,7 @@
         <v>29.173455047623001</v>
       </c>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A357" s="1">
         <v>44600</v>
       </c>
@@ -14883,7 +14894,7 @@
         <v>27.6620245651823</v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A358" s="1">
         <v>44601</v>
       </c>
@@ -14900,7 +14911,7 @@
         <v>26.615497910002301</v>
       </c>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A359" s="1">
         <v>44602</v>
       </c>
@@ -14917,7 +14928,7 @@
         <v>25.676457750832299</v>
       </c>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A360" s="1">
         <v>44603</v>
       </c>
@@ -14934,7 +14945,7 @@
         <v>24.7159268278611</v>
       </c>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A361" s="1">
         <v>44606</v>
       </c>
@@ -14951,7 +14962,7 @@
         <v>24.913831214752399</v>
       </c>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A362" s="1">
         <v>44607</v>
       </c>
@@ -14968,7 +14979,7 @@
         <v>25.2687452558019</v>
       </c>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A363" s="1">
         <v>44608</v>
       </c>
@@ -14985,7 +14996,7 @@
         <v>25.26505559864</v>
       </c>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A364" s="1">
         <v>44609</v>
       </c>
@@ -15002,7 +15013,7 @@
         <v>25.279551578790802</v>
       </c>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A365" s="1">
         <v>44610</v>
       </c>
@@ -15019,7 +15030,7 @@
         <v>25.925140123281899</v>
       </c>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A366" s="1">
         <v>44614</v>
       </c>
@@ -15036,7 +15047,7 @@
         <v>26.617483964001099</v>
       </c>
     </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A367" s="1">
         <v>44615</v>
       </c>
@@ -15053,7 +15064,7 @@
         <v>27.3009991220597</v>
       </c>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A368" s="1">
         <v>44616</v>
       </c>
@@ -15070,7 +15081,7 @@
         <v>27.097812883155399</v>
       </c>
     </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A369" s="1">
         <v>44617</v>
       </c>
@@ -15087,7 +15098,7 @@
         <v>26.270831248290602</v>
       </c>
     </row>
-    <row r="370" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A370" s="1">
         <v>44620</v>
       </c>
@@ -15104,7 +15115,7 @@
         <v>24.988157396879</v>
       </c>
     </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A371" s="1">
         <v>44621</v>
       </c>
@@ -15121,7 +15132,7 @@
         <v>24.061465219004599</v>
       </c>
     </row>
-    <row r="372" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A372" s="1">
         <v>44622</v>
       </c>
@@ -15138,7 +15149,7 @@
         <v>23.167749467358899</v>
       </c>
     </row>
-    <row r="373" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A373" s="1">
         <v>44623</v>
       </c>
@@ -15155,7 +15166,7 @@
         <v>22.4782504615563</v>
       </c>
     </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A374" s="1">
         <v>44624</v>
       </c>
@@ -15172,7 +15183,7 @@
         <v>21.795702573848001</v>
       </c>
     </row>
-    <row r="375" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A375" s="1">
         <v>44627</v>
       </c>
@@ -15189,7 +15200,7 @@
         <v>21.003892143032001</v>
       </c>
     </row>
-    <row r="376" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A376" s="1">
         <v>44628</v>
       </c>
@@ -15206,7 +15217,7 @@
         <v>20.687634405189399</v>
       </c>
     </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A377" s="1">
         <v>44629</v>
       </c>
@@ -15223,7 +15234,7 @@
         <v>21.292302806136401</v>
       </c>
     </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A378" s="1">
         <v>44630</v>
       </c>
@@ -15240,7 +15251,7 @@
         <v>22.3171392559785</v>
       </c>
     </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A379" s="1">
         <v>44631</v>
       </c>
@@ -15257,7 +15268,7 @@
         <v>23.234837606249702</v>
       </c>
     </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A380" s="1">
         <v>44634</v>
       </c>
@@ -15274,7 +15285,7 @@
         <v>23.9706117579961</v>
       </c>
     </row>
-    <row r="381" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A381" s="1">
         <v>44635</v>
       </c>
@@ -15291,7 +15302,7 @@
         <v>24.226158265629799</v>
       </c>
     </row>
-    <row r="382" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A382" s="1">
         <v>44636</v>
       </c>
@@ -15308,7 +15319,7 @@
         <v>23.410355976005899</v>
       </c>
     </row>
-    <row r="383" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A383" s="1">
         <v>44637</v>
       </c>
@@ -15325,7 +15336,7 @@
         <v>22.567778903036</v>
       </c>
     </row>
-    <row r="384" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A384" s="1">
         <v>44638</v>
       </c>
@@ -15342,7 +15353,7 @@
         <v>21.113670892872001</v>
       </c>
     </row>
-    <row r="385" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A385" s="1">
         <v>44641</v>
       </c>
@@ -15359,7 +15370,7 @@
         <v>19.790737689009099</v>
       </c>
     </row>
-    <row r="386" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A386" s="1">
         <v>44642</v>
       </c>
@@ -15376,7 +15387,7 @@
         <v>18.9474138840202</v>
       </c>
     </row>
-    <row r="387" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A387" s="1">
         <v>44643</v>
       </c>
@@ -15393,7 +15404,7 @@
         <v>18.4731310843109</v>
       </c>
     </row>
-    <row r="388" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A388" s="1">
         <v>44644</v>
       </c>
@@ -15410,7 +15421,7 @@
         <v>18.985241527545401</v>
       </c>
     </row>
-    <row r="389" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A389" s="1">
         <v>44645</v>
       </c>
@@ -15427,7 +15438,7 @@
         <v>19.543013499372101</v>
       </c>
     </row>
-    <row r="390" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A390" s="1">
         <v>44648</v>
       </c>
@@ -15444,7 +15455,7 @@
         <v>20.377575215669001</v>
       </c>
     </row>
-    <row r="391" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A391" s="1">
         <v>44649</v>
       </c>
@@ -15461,7 +15472,7 @@
         <v>21.495473725297401</v>
       </c>
     </row>
-    <row r="392" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A392" s="2">
         <v>44650</v>
       </c>
@@ -15478,7 +15489,7 @@
         <v>23.0866034177633</v>
       </c>
     </row>
-    <row r="393" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A393" s="2">
         <v>44651</v>
       </c>
@@ -15495,7 +15506,7 @@
         <v>23.6181051360807</v>
       </c>
     </row>
-    <row r="394" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A394" s="1">
         <v>44652</v>
       </c>
@@ -15512,7 +15523,7 @@
         <v>22.498825878657001</v>
       </c>
     </row>
-    <row r="395" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A395" s="1">
         <v>44655</v>
       </c>
@@ -15529,7 +15540,7 @@
         <v>21.1457862114394</v>
       </c>
     </row>
-    <row r="396" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A396" s="1">
         <v>44656</v>
       </c>
@@ -15546,7 +15557,7 @@
         <v>19.7492121013907</v>
       </c>
     </row>
-    <row r="397" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A397" s="1">
         <v>44657</v>
       </c>
@@ -15563,7 +15574,7 @@
         <v>18.783905384125799</v>
       </c>
     </row>
-    <row r="398" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A398" s="1">
         <v>44658</v>
       </c>
@@ -15580,7 +15591,7 @@
         <v>18.333701066682099</v>
       </c>
     </row>
-    <row r="399" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A399" s="1">
         <v>44659</v>
       </c>
@@ -15597,7 +15608,7 @@
         <v>18.366630656409299</v>
       </c>
     </row>
-    <row r="400" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A400" s="1">
         <v>44662</v>
       </c>
@@ -15614,7 +15625,7 @@
         <v>19.1491138198915</v>
       </c>
     </row>
-    <row r="401" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A401" s="1">
         <v>44663</v>
       </c>
@@ -15631,7 +15642,7 @@
         <v>19.6036837421508</v>
       </c>
     </row>
-    <row r="402" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A402" s="1">
         <v>44664</v>
       </c>
@@ -15648,7 +15659,7 @@
         <v>20.0232867473133</v>
       </c>
     </row>
-    <row r="403" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A403" s="1">
         <v>44665</v>
       </c>
@@ -15665,7 +15676,7 @@
         <v>21.0061388827136</v>
       </c>
     </row>
-    <row r="404" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A404" s="1">
         <v>44669</v>
       </c>
@@ -15682,7 +15693,7 @@
         <v>21.8804967991104</v>
       </c>
     </row>
-    <row r="405" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A405" s="1">
         <v>44670</v>
       </c>
@@ -15699,7 +15710,7 @@
         <v>21.038014230732799</v>
       </c>
     </row>
-    <row r="406" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A406" s="2">
         <v>44671</v>
       </c>
@@ -15716,7 +15727,7 @@
         <v>19.860955373420801</v>
       </c>
     </row>
-    <row r="407" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A407" s="1">
         <v>44672</v>
       </c>
@@ -15733,7 +15744,7 @@
         <v>18.529807918727499</v>
       </c>
     </row>
-    <row r="408" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A408" s="1">
         <v>44673</v>
       </c>
@@ -15750,7 +15761,7 @@
         <v>17.715590295991799</v>
       </c>
     </row>
-    <row r="409" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A409" s="1">
         <v>44676</v>
       </c>
@@ -15767,7 +15778,7 @@
         <v>17.404932620989399</v>
       </c>
     </row>
-    <row r="410" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A410" s="1">
         <v>44677</v>
       </c>
@@ -15784,7 +15795,7 @@
         <v>17.564404312851799</v>
       </c>
     </row>
-    <row r="411" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A411" s="1">
         <v>44678</v>
       </c>
@@ -15801,7 +15812,7 @@
         <v>17.900862031989401</v>
       </c>
     </row>
-    <row r="412" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A412" s="1">
         <v>44679</v>
       </c>
@@ -15818,7 +15829,7 @@
         <v>17.642074066261198</v>
       </c>
     </row>
-    <row r="413" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A413" s="1">
         <v>44680</v>
       </c>
@@ -15835,7 +15846,7 @@
         <v>17.774345919429202</v>
       </c>
     </row>
-    <row r="414" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A414" s="1">
         <v>44683</v>
       </c>
@@ -15852,7 +15863,7 @@
         <v>17.896443014661099</v>
       </c>
     </row>
-    <row r="415" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A415" s="1">
         <v>44684</v>
       </c>
@@ -15869,7 +15880,7 @@
         <v>18.1409077968429</v>
       </c>
     </row>
-    <row r="416" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A416" s="1">
         <v>44685</v>
       </c>
@@ -15886,7 +15897,7 @@
         <v>17.710289975155199</v>
       </c>
     </row>
-    <row r="417" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A417" s="1">
         <v>44686</v>
       </c>
@@ -15903,7 +15914,7 @@
         <v>16.669151834753698</v>
       </c>
     </row>
-    <row r="418" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A418" s="1">
         <v>44687</v>
       </c>
@@ -15920,7 +15931,7 @@
         <v>16.008897354855801</v>
       </c>
     </row>
-    <row r="419" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A419" s="1">
         <v>44690</v>
       </c>
@@ -15937,7 +15948,7 @@
         <v>15.5501703085808</v>
       </c>
     </row>
-    <row r="420" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A420" s="1">
         <v>44691</v>
       </c>
@@ -15954,7 +15965,7 @@
         <v>15.2503647346657</v>
       </c>
     </row>
-    <row r="421" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A421" s="1">
         <v>44692</v>
       </c>
@@ -15971,7 +15982,7 @@
         <v>15.396541968257401</v>
       </c>
     </row>
-    <row r="422" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A422" s="1">
         <v>44693</v>
       </c>
@@ -15988,7 +15999,7 @@
         <v>16.081065030888599</v>
       </c>
     </row>
-    <row r="423" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A423" s="1">
         <v>44694</v>
       </c>
@@ -16005,7 +16016,7 @@
         <v>16.391278707350299</v>
       </c>
     </row>
-    <row r="424" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A424" s="1">
         <v>44697</v>
       </c>
@@ -16022,7 +16033,7 @@
         <v>16.057355349542998</v>
       </c>
     </row>
-    <row r="425" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A425" s="1">
         <v>44698</v>
       </c>
@@ -16039,7 +16050,7 @@
         <v>16.0521154627443</v>
       </c>
     </row>
-    <row r="426" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A426" s="1">
         <v>44699</v>
       </c>
@@ -16056,7 +16067,7 @@
         <v>16.6111939867803</v>
       </c>
     </row>
-    <row r="427" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A427" s="1">
         <v>44700</v>
       </c>
@@ -16073,7 +16084,7 @@
         <v>17.0234721126319</v>
       </c>
     </row>
-    <row r="428" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A428" s="1">
         <v>44701</v>
       </c>
@@ -16090,7 +16101,7 @@
         <v>17.2594939350159</v>
       </c>
     </row>
-    <row r="429" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A429" s="1">
         <v>44704</v>
       </c>
@@ -16107,7 +16118,7 @@
         <v>17.4773602326012</v>
       </c>
     </row>
-    <row r="430" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A430" s="1">
         <v>44705</v>
       </c>
@@ -16124,7 +16135,7 @@
         <v>17.872063869780199</v>
       </c>
     </row>
-    <row r="431" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A431" s="1">
         <v>44706</v>
       </c>
@@ -16141,7 +16152,7 @@
         <v>18.249784410107502</v>
       </c>
     </row>
-    <row r="432" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A432" s="1">
         <v>44707</v>
       </c>
@@ -16158,7 +16169,7 @@
         <v>17.684408476798701</v>
       </c>
     </row>
-    <row r="433" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A433" s="1">
         <v>44708</v>
       </c>
@@ -16175,7 +16186,7 @@
         <v>17.0827635233561</v>
       </c>
     </row>
-    <row r="434" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A434" s="1">
         <v>44712</v>
       </c>
@@ -16192,7 +16203,7 @@
         <v>16.891920633676801</v>
       </c>
     </row>
-    <row r="435" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A435" s="1">
         <v>44713</v>
       </c>
@@ -16209,7 +16220,7 @@
         <v>16.2866108733038</v>
       </c>
     </row>
-    <row r="436" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A436" s="1">
         <v>44714</v>
       </c>
@@ -16226,7 +16237,7 @@
         <v>15.801309998359001</v>
       </c>
     </row>
-    <row r="437" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A437" s="1">
         <v>44715</v>
       </c>
@@ -16243,7 +16254,7 @@
         <v>14.8812986270477</v>
       </c>
     </row>
-    <row r="438" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A438" s="1">
         <v>44718</v>
       </c>
@@ -16260,7 +16271,7 @@
         <v>14.728357760366199</v>
       </c>
     </row>
-    <row r="439" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A439" s="1">
         <v>44719</v>
       </c>
@@ -16277,7 +16288,7 @@
         <v>14.9684590937094</v>
       </c>
     </row>
-    <row r="440" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A440" s="1">
         <v>44720</v>
       </c>
@@ -16294,7 +16305,7 @@
         <v>16.280457065887202</v>
       </c>
     </row>
-    <row r="441" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A441" s="1">
         <v>44721</v>
       </c>
@@ -16311,7 +16322,7 @@
         <v>17.811498661765899</v>
       </c>
     </row>
-    <row r="442" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A442" s="1">
         <v>44722</v>
       </c>
@@ -16328,7 +16339,7 @@
         <v>19.516036416927999</v>
       </c>
     </row>
-    <row r="443" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A443" s="1">
         <v>44725</v>
       </c>
@@ -16345,7 +16356,7 @@
         <v>21.046290198700198</v>
       </c>
     </row>
-    <row r="444" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A444" s="1">
         <v>44726</v>
       </c>
@@ -16362,7 +16373,7 @@
         <v>21.861947254220301</v>
       </c>
     </row>
-    <row r="445" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A445" s="1">
         <v>44727</v>
       </c>
@@ -16379,7 +16390,7 @@
         <v>21.632537519547501</v>
       </c>
     </row>
-    <row r="446" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A446" s="1">
         <v>44728</v>
       </c>
@@ -16396,7 +16407,7 @@
         <v>21.7579770916199</v>
       </c>
     </row>
-    <row r="447" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A447" s="1">
         <v>44729</v>
       </c>
@@ -16413,7 +16424,7 @@
         <v>21.9555272193262</v>
       </c>
     </row>
-    <row r="448" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A448" s="1">
         <v>44733</v>
       </c>
@@ -16430,7 +16441,7 @@
         <v>22.137881183362801</v>
       </c>
     </row>
-    <row r="449" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A449" s="1">
         <v>44734</v>
       </c>
@@ -16447,7 +16458,7 @@
         <v>22.282622450856799</v>
       </c>
     </row>
-    <row r="450" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A450" s="1">
         <v>44735</v>
       </c>
@@ -16464,7 +16475,7 @@
         <v>22.638473497561598</v>
       </c>
     </row>
-    <row r="451" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A451" s="1">
         <v>44736</v>
       </c>
@@ -16481,7 +16492,7 @@
         <v>22.438632857791301</v>
       </c>
     </row>
-    <row r="452" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A452" s="1">
         <v>44739</v>
       </c>
@@ -16498,7 +16509,7 @@
         <v>22.651006981690902</v>
       </c>
     </row>
-    <row r="453" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A453" s="1">
         <v>44740</v>
       </c>
@@ -16515,7 +16526,7 @@
         <v>23.453672368341099</v>
       </c>
     </row>
-    <row r="454" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A454" s="1">
         <v>44741</v>
       </c>
@@ -16532,7 +16543,7 @@
         <v>24.671937513344801</v>
       </c>
     </row>
-    <row r="455" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A455" s="1">
         <v>44742</v>
       </c>
@@ -16549,7 +16560,7 @@
         <v>25.862421656135901</v>
       </c>
     </row>
-    <row r="456" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A456" s="1">
         <v>44743</v>
       </c>
@@ -16566,7 +16577,7 @@
         <v>27.283813701338399</v>
       </c>
     </row>
-    <row r="457" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A457" s="1">
         <v>44747</v>
       </c>
@@ -16583,7 +16594,7 @@
         <v>28.090079255227099</v>
       </c>
     </row>
-    <row r="458" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A458" s="1">
         <v>44748</v>
       </c>
@@ -16600,7 +16611,7 @@
         <v>28.614967537533001</v>
       </c>
     </row>
-    <row r="459" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A459" s="1">
         <v>44749</v>
       </c>
@@ -16617,7 +16628,7 @@
         <v>28.556310485218901</v>
       </c>
     </row>
-    <row r="460" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A460" s="1">
         <v>44750</v>
       </c>
@@ -16634,7 +16645,7 @@
         <v>28.650012536091701</v>
       </c>
     </row>
-    <row r="461" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A461" s="1">
         <v>44753</v>
       </c>
@@ -16651,7 +16662,7 @@
         <v>28.920811191664001</v>
       </c>
     </row>
-    <row r="462" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A462" s="1">
         <v>44754</v>
       </c>
@@ -16668,7 +16679,7 @@
         <v>29.278248007384502</v>
       </c>
     </row>
-    <row r="463" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A463" s="1">
         <v>44755</v>
       </c>
@@ -16685,7 +16696,7 @@
         <v>29.035547019114698</v>
       </c>
     </row>
-    <row r="464" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A464" s="1">
         <v>44756</v>
       </c>
@@ -16702,7 +16713,7 @@
         <v>28.047715563609501</v>
       </c>
     </row>
-    <row r="465" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A465" s="1">
         <v>44757</v>
       </c>
@@ -16719,7 +16730,7 @@
         <v>27.107197101028301</v>
       </c>
     </row>
-    <row r="466" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A466" s="1">
         <v>44760</v>
       </c>
@@ -16736,7 +16747,7 @@
         <v>26.596159015351699</v>
       </c>
     </row>
-    <row r="467" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A467" s="1">
         <v>44761</v>
       </c>
@@ -16753,7 +16764,7 @@
         <v>26.479392919432499</v>
       </c>
     </row>
-    <row r="468" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A468" s="1">
         <v>44762</v>
       </c>
@@ -16770,7 +16781,7 @@
         <v>26.6678353834345</v>
       </c>
     </row>
-    <row r="469" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A469" s="1">
         <v>44763</v>
       </c>
@@ -16787,7 +16798,7 @@
         <v>26.952046806343699</v>
       </c>
     </row>
-    <row r="470" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A470" s="1">
         <v>44764</v>
       </c>
@@ -16804,7 +16815,7 @@
         <v>26.1663815845871</v>
       </c>
     </row>
-    <row r="471" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A471" s="1">
         <v>44767</v>
       </c>
@@ -16821,7 +16832,7 @@
         <v>24.667666006182799</v>
       </c>
     </row>
-    <row r="472" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A472" s="1">
         <v>44768</v>
       </c>
@@ -16838,7 +16849,7 @@
         <v>23.520865655079099</v>
       </c>
     </row>
-    <row r="473" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A473" s="1">
         <v>44769</v>
       </c>
@@ -16855,7 +16866,7 @@
         <v>23.073500886441799</v>
       </c>
     </row>
-    <row r="474" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A474" s="1">
         <v>44770</v>
       </c>
@@ -16872,7 +16883,7 @@
         <v>22.550499517190602</v>
       </c>
     </row>
-    <row r="475" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A475" s="1">
         <v>44771</v>
       </c>
@@ -16889,7 +16900,7 @@
         <v>22.939870876771401</v>
       </c>
     </row>
-    <row r="476" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A476" s="1">
         <v>44774</v>
       </c>
@@ -16906,7 +16917,7 @@
         <v>22.279756049859301</v>
       </c>
     </row>
-    <row r="477" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A477" s="1">
         <v>44775</v>
       </c>
@@ -16923,7 +16934,7 @@
         <v>21.3719082921451</v>
       </c>
     </row>
-    <row r="478" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A478" s="1">
         <v>44776</v>
       </c>
@@ -16940,7 +16951,7 @@
         <v>20.8862905967299</v>
       </c>
     </row>
-    <row r="479" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A479" s="1">
         <v>44777</v>
       </c>
@@ -16957,7 +16968,7 @@
         <v>21.065883583145599</v>
       </c>
     </row>
-    <row r="480" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A480" s="1">
         <v>44778</v>
       </c>
@@ -16974,7 +16985,7 @@
         <v>21.2959980881276</v>
       </c>
     </row>
-    <row r="481" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A481" s="1">
         <v>44781</v>
       </c>
@@ -16991,7 +17002,7 @@
         <v>21.3418448533766</v>
       </c>
     </row>
-    <row r="482" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A482" s="1">
         <v>44782</v>
       </c>
@@ -17008,7 +17019,7 @@
         <v>21.106875359095401</v>
       </c>
     </row>
-    <row r="483" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A483" s="1">
         <v>44783</v>
       </c>
@@ -17025,7 +17036,7 @@
         <v>20.593543850193502</v>
       </c>
     </row>
-    <row r="484" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A484" s="1">
         <v>44784</v>
       </c>
@@ -17042,7 +17053,7 @@
         <v>19.651040554468899</v>
       </c>
     </row>
-    <row r="485" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A485" s="1">
         <v>44785</v>
       </c>
@@ -17059,7 +17070,7 @@
         <v>19.237709080052099</v>
       </c>
     </row>
-    <row r="486" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A486" s="1">
         <v>44788</v>
       </c>
@@ -17076,7 +17087,7 @@
         <v>18.547474317142999</v>
       </c>
     </row>
-    <row r="487" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A487" s="1">
         <v>44789</v>
       </c>
@@ -17093,7 +17104,7 @@
         <v>18.5246043671847</v>
       </c>
     </row>
-    <row r="488" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A488" s="1">
         <v>44790</v>
       </c>
@@ -17110,7 +17121,7 @@
         <v>18.2172210338281</v>
       </c>
     </row>
-    <row r="489" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A489" s="1">
         <v>44791</v>
       </c>
@@ -17127,7 +17138,7 @@
         <v>17.774383037522099</v>
       </c>
     </row>
-    <row r="490" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A490" s="1">
         <v>44792</v>
       </c>
@@ -17144,7 +17155,7 @@
         <v>17.833138492282899</v>
       </c>
     </row>
-    <row r="491" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A491" s="1">
         <v>44795</v>
       </c>
@@ -17161,7 +17172,7 @@
         <v>18.5709577533082</v>
       </c>
     </row>
-    <row r="492" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A492" s="1">
         <v>44796</v>
       </c>
@@ -17178,7 +17189,7 @@
         <v>19.316358050237501</v>
       </c>
     </row>
-    <row r="493" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A493" s="1">
         <v>44797</v>
       </c>
@@ -17195,7 +17206,7 @@
         <v>19.966751685649299</v>
       </c>
     </row>
-    <row r="494" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A494" s="1">
         <v>44798</v>
       </c>
@@ -17212,7 +17223,7 @@
         <v>20.158733044033202</v>
       </c>
     </row>
-    <row r="495" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A495" s="1">
         <v>44799</v>
       </c>
@@ -17229,7 +17240,7 @@
         <v>20.4942328435951</v>
       </c>
     </row>
-    <row r="496" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A496" s="1">
         <v>44802</v>
       </c>
@@ -17246,7 +17257,7 @@
         <v>20.4857876875401</v>
       </c>
     </row>
-    <row r="497" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A497" s="1">
         <v>44803</v>
       </c>
@@ -17263,7 +17274,7 @@
         <v>20.7419232064086</v>
       </c>
     </row>
-    <row r="498" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A498" s="1">
         <v>44804</v>
       </c>
@@ -17280,7 +17291,7 @@
         <v>20.937929088357699</v>
       </c>
     </row>
-    <row r="499" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="499" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A499" s="1">
         <v>44805</v>
       </c>
@@ -17297,7 +17308,7 @@
         <v>21.246677841335099</v>
       </c>
     </row>
-    <row r="500" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="500" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A500" s="1">
         <v>44806</v>
       </c>
@@ -17314,7 +17325,7 @@
         <v>21.3311927138481</v>
       </c>
     </row>
-    <row r="501" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="501" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A501" s="1">
         <v>44810</v>
       </c>
@@ -17331,7 +17342,7 @@
         <v>21.498914064205898</v>
       </c>
     </row>
-    <row r="502" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="502" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A502" s="1">
         <v>44811</v>
       </c>
@@ -17348,7 +17359,7 @@
         <v>21.968856778994802</v>
       </c>
     </row>
-    <row r="503" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="503" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A503" s="1">
         <v>44812</v>
       </c>

</xml_diff>